<commit_message>
Creating Observations and refining FSH files
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-HIV-patient.xlsx
+++ b/output/StructureDefinition-HIV-patient.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1708" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="339">
   <si>
     <t>Path</t>
   </si>
@@ -516,10 +516,7 @@
     <t>required</t>
   </si>
   <si>
-    <t>The gender of a person used for administrative purposes.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/administrative-gender|4.0.1</t>
+    <t>http://example.org/fhir/fish/ValueSet/HIVGender</t>
   </si>
   <si>
     <t>player[classCode=PSN|ANM and determinerCode=INSTANCE]/administrativeGender</t>
@@ -845,6 +842,12 @@
   </si>
   <si>
     <t>Needed to address the person correctly.</t>
+  </si>
+  <si>
+    <t>The gender of a person used for administrative purposes.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/administrative-gender|4.0.1</t>
   </si>
   <si>
     <t>NK1-15</t>
@@ -3060,11 +3063,9 @@
       <c r="W16" t="s" s="2">
         <v>157</v>
       </c>
-      <c r="X16" t="s" s="2">
+      <c r="X16" s="2"/>
+      <c r="Y16" t="s" s="2">
         <v>158</v>
-      </c>
-      <c r="Y16" t="s" s="2">
-        <v>159</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>44</v>
@@ -3097,16 +3098,16 @@
         <v>63</v>
       </c>
       <c r="AJ16" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="AK16" t="s" s="2">
         <v>160</v>
       </c>
-      <c r="AK16" t="s" s="2">
+      <c r="AL16" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM16" t="s" s="2">
         <v>161</v>
-      </c>
-      <c r="AL16" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM16" t="s" s="2">
-        <v>162</v>
       </c>
       <c r="AN16" t="s" s="2">
         <v>44</v>
@@ -3114,7 +3115,7 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3137,19 +3138,19 @@
         <v>52</v>
       </c>
       <c r="J17" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="K17" t="s" s="2">
         <v>164</v>
       </c>
-      <c r="K17" t="s" s="2">
+      <c r="L17" t="s" s="2">
         <v>165</v>
       </c>
-      <c r="L17" t="s" s="2">
+      <c r="M17" t="s" s="2">
         <v>166</v>
       </c>
-      <c r="M17" t="s" s="2">
+      <c r="N17" t="s" s="2">
         <v>167</v>
-      </c>
-      <c r="N17" t="s" s="2">
-        <v>168</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>44</v>
@@ -3198,7 +3199,7 @@
         <v>44</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>42</v>
@@ -3213,24 +3214,24 @@
         <v>63</v>
       </c>
       <c r="AJ17" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="AK17" t="s" s="2">
         <v>169</v>
       </c>
-      <c r="AK17" t="s" s="2">
+      <c r="AL17" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM17" t="s" s="2">
         <v>170</v>
       </c>
-      <c r="AL17" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM17" t="s" s="2">
+      <c r="AN17" t="s" s="2">
         <v>171</v>
-      </c>
-      <c r="AN17" t="s" s="2">
-        <v>172</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3253,19 +3254,19 @@
         <v>52</v>
       </c>
       <c r="J18" t="s" s="2">
+        <v>173</v>
+      </c>
+      <c r="K18" t="s" s="2">
         <v>174</v>
       </c>
-      <c r="K18" t="s" s="2">
+      <c r="L18" t="s" s="2">
         <v>175</v>
       </c>
-      <c r="L18" t="s" s="2">
+      <c r="M18" t="s" s="2">
         <v>176</v>
       </c>
-      <c r="M18" t="s" s="2">
+      <c r="N18" t="s" s="2">
         <v>177</v>
-      </c>
-      <c r="N18" t="s" s="2">
-        <v>178</v>
       </c>
       <c r="O18" t="s" s="2">
         <v>44</v>
@@ -3314,7 +3315,7 @@
         <v>44</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>42</v>
@@ -3329,7 +3330,7 @@
         <v>63</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AK18" t="s" s="2">
         <v>132</v>
@@ -3338,7 +3339,7 @@
         <v>44</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AN18" t="s" s="2">
         <v>44</v>
@@ -3346,7 +3347,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3369,19 +3370,19 @@
         <v>52</v>
       </c>
       <c r="J19" t="s" s="2">
+        <v>181</v>
+      </c>
+      <c r="K19" t="s" s="2">
         <v>182</v>
       </c>
-      <c r="K19" t="s" s="2">
+      <c r="L19" t="s" s="2">
         <v>183</v>
       </c>
-      <c r="L19" t="s" s="2">
+      <c r="M19" t="s" s="2">
         <v>184</v>
       </c>
-      <c r="M19" t="s" s="2">
+      <c r="N19" t="s" s="2">
         <v>185</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>186</v>
       </c>
       <c r="O19" t="s" s="2">
         <v>44</v>
@@ -3430,7 +3431,7 @@
         <v>44</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>42</v>
@@ -3445,16 +3446,16 @@
         <v>63</v>
       </c>
       <c r="AJ19" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="AK19" t="s" s="2">
         <v>187</v>
       </c>
-      <c r="AK19" t="s" s="2">
+      <c r="AL19" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM19" t="s" s="2">
         <v>188</v>
-      </c>
-      <c r="AL19" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM19" t="s" s="2">
-        <v>189</v>
       </c>
       <c r="AN19" t="s" s="2">
         <v>44</v>
@@ -3462,7 +3463,7 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3485,17 +3486,17 @@
         <v>44</v>
       </c>
       <c r="J20" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="K20" t="s" s="2">
         <v>191</v>
       </c>
-      <c r="K20" t="s" s="2">
+      <c r="L20" t="s" s="2">
         <v>192</v>
-      </c>
-      <c r="L20" t="s" s="2">
-        <v>193</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" t="s" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>44</v>
@@ -3520,14 +3521,14 @@
         <v>44</v>
       </c>
       <c r="W20" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="X20" t="s" s="2">
         <v>195</v>
       </c>
-      <c r="X20" t="s" s="2">
+      <c r="Y20" t="s" s="2">
         <v>196</v>
       </c>
-      <c r="Y20" t="s" s="2">
-        <v>197</v>
-      </c>
       <c r="Z20" t="s" s="2">
         <v>44</v>
       </c>
@@ -3544,7 +3545,7 @@
         <v>44</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>42</v>
@@ -3559,16 +3560,16 @@
         <v>63</v>
       </c>
       <c r="AJ20" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="AK20" t="s" s="2">
         <v>198</v>
       </c>
-      <c r="AK20" t="s" s="2">
+      <c r="AL20" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM20" t="s" s="2">
         <v>199</v>
-      </c>
-      <c r="AL20" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM20" t="s" s="2">
-        <v>200</v>
       </c>
       <c r="AN20" t="s" s="2">
         <v>44</v>
@@ -3576,7 +3577,7 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3599,19 +3600,19 @@
         <v>44</v>
       </c>
       <c r="J21" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="K21" t="s" s="2">
         <v>202</v>
       </c>
-      <c r="K21" t="s" s="2">
+      <c r="L21" t="s" s="2">
         <v>203</v>
       </c>
-      <c r="L21" t="s" s="2">
+      <c r="M21" t="s" s="2">
         <v>204</v>
       </c>
-      <c r="M21" t="s" s="2">
+      <c r="N21" t="s" s="2">
         <v>205</v>
-      </c>
-      <c r="N21" t="s" s="2">
-        <v>206</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>44</v>
@@ -3660,7 +3661,7 @@
         <v>44</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>42</v>
@@ -3675,7 +3676,7 @@
         <v>63</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>132</v>
@@ -3684,7 +3685,7 @@
         <v>44</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AN21" t="s" s="2">
         <v>44</v>
@@ -3692,7 +3693,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3715,19 +3716,19 @@
         <v>44</v>
       </c>
       <c r="J22" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="K22" t="s" s="2">
         <v>210</v>
       </c>
-      <c r="K22" t="s" s="2">
+      <c r="L22" t="s" s="2">
         <v>211</v>
       </c>
-      <c r="L22" t="s" s="2">
+      <c r="M22" t="s" s="2">
         <v>212</v>
       </c>
-      <c r="M22" t="s" s="2">
+      <c r="N22" t="s" s="2">
         <v>213</v>
-      </c>
-      <c r="N22" t="s" s="2">
-        <v>214</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>44</v>
@@ -3776,7 +3777,7 @@
         <v>44</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>42</v>
@@ -3791,7 +3792,7 @@
         <v>63</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>132</v>
@@ -3800,7 +3801,7 @@
         <v>44</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AN22" t="s" s="2">
         <v>44</v>
@@ -3808,7 +3809,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3831,19 +3832,19 @@
         <v>44</v>
       </c>
       <c r="J23" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="K23" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="K23" t="s" s="2">
+      <c r="L23" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="L23" t="s" s="2">
+      <c r="M23" t="s" s="2">
         <v>220</v>
       </c>
-      <c r="M23" t="s" s="2">
+      <c r="N23" t="s" s="2">
         <v>221</v>
-      </c>
-      <c r="N23" t="s" s="2">
-        <v>222</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>44</v>
@@ -3892,7 +3893,7 @@
         <v>44</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>42</v>
@@ -3904,10 +3905,10 @@
         <v>44</v>
       </c>
       <c r="AI23" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="AJ23" t="s" s="2">
         <v>223</v>
-      </c>
-      <c r="AJ23" t="s" s="2">
-        <v>224</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>132</v>
@@ -3924,7 +3925,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3950,10 +3951,10 @@
         <v>53</v>
       </c>
       <c r="K24" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="L24" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="L24" t="s" s="2">
-        <v>227</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -4004,7 +4005,7 @@
         <v>44</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>42</v>
@@ -4036,7 +4037,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4062,10 +4063,10 @@
         <v>96</v>
       </c>
       <c r="K25" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="L25" t="s" s="2">
         <v>230</v>
-      </c>
-      <c r="L25" t="s" s="2">
-        <v>231</v>
       </c>
       <c r="M25" t="s" s="2">
         <v>112</v>
@@ -4118,7 +4119,7 @@
         <v>44</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>42</v>
@@ -4150,11 +4151,11 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
@@ -4176,10 +4177,10 @@
         <v>96</v>
       </c>
       <c r="K26" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="L26" t="s" s="2">
         <v>235</v>
-      </c>
-      <c r="L26" t="s" s="2">
-        <v>236</v>
       </c>
       <c r="M26" t="s" s="2">
         <v>112</v>
@@ -4234,7 +4235,7 @@
         <v>44</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>42</v>
@@ -4266,7 +4267,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4289,17 +4290,17 @@
         <v>44</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K27" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="L27" t="s" s="2">
         <v>239</v>
-      </c>
-      <c r="L27" t="s" s="2">
-        <v>240</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" t="s" s="2">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>44</v>
@@ -4324,14 +4325,14 @@
         <v>44</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="X27" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="Y27" t="s" s="2">
         <v>242</v>
       </c>
-      <c r="Y27" t="s" s="2">
-        <v>243</v>
-      </c>
       <c r="Z27" t="s" s="2">
         <v>44</v>
       </c>
@@ -4348,7 +4349,7 @@
         <v>44</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>42</v>
@@ -4363,7 +4364,7 @@
         <v>63</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AK27" t="s" s="2">
         <v>132</v>
@@ -4372,7 +4373,7 @@
         <v>44</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>44</v>
@@ -4380,7 +4381,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4406,14 +4407,14 @@
         <v>135</v>
       </c>
       <c r="K28" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="L28" t="s" s="2">
         <v>247</v>
-      </c>
-      <c r="L28" t="s" s="2">
-        <v>248</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" t="s" s="2">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="O28" t="s" s="2">
         <v>44</v>
@@ -4462,7 +4463,7 @@
         <v>44</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>42</v>
@@ -4486,7 +4487,7 @@
         <v>44</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>44</v>
@@ -4494,7 +4495,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4520,13 +4521,13 @@
         <v>144</v>
       </c>
       <c r="K29" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="L29" t="s" s="2">
         <v>252</v>
       </c>
-      <c r="L29" t="s" s="2">
+      <c r="M29" t="s" s="2">
         <v>253</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>254</v>
       </c>
       <c r="N29" t="s" s="2">
         <v>148</v>
@@ -4578,7 +4579,7 @@
         <v>44</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>42</v>
@@ -4602,7 +4603,7 @@
         <v>44</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>44</v>
@@ -4610,7 +4611,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4633,17 +4634,17 @@
         <v>44</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K30" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="L30" t="s" s="2">
         <v>257</v>
-      </c>
-      <c r="L30" t="s" s="2">
-        <v>258</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" t="s" s="2">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>44</v>
@@ -4692,7 +4693,7 @@
         <v>44</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>42</v>
@@ -4707,7 +4708,7 @@
         <v>63</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AK30" t="s" s="2">
         <v>132</v>
@@ -4716,7 +4717,7 @@
         <v>44</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>44</v>
@@ -4724,7 +4725,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4753,11 +4754,11 @@
         <v>153</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" t="s" s="2">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="O31" t="s" s="2">
         <v>44</v>
@@ -4785,10 +4786,10 @@
         <v>157</v>
       </c>
       <c r="X31" t="s" s="2">
-        <v>158</v>
+        <v>263</v>
       </c>
       <c r="Y31" t="s" s="2">
-        <v>159</v>
+        <v>264</v>
       </c>
       <c r="Z31" t="s" s="2">
         <v>44</v>
@@ -4806,7 +4807,7 @@
         <v>44</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>42</v>
@@ -4821,7 +4822,7 @@
         <v>63</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>132</v>
@@ -4830,7 +4831,7 @@
         <v>44</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>44</v>
@@ -4838,7 +4839,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4861,17 +4862,17 @@
         <v>44</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>44</v>
@@ -4920,7 +4921,7 @@
         <v>44</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>42</v>
@@ -4929,13 +4930,13 @@
         <v>51</v>
       </c>
       <c r="AH32" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AI32" t="s" s="2">
         <v>63</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>132</v>
@@ -4944,7 +4945,7 @@
         <v>44</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>44</v>
@@ -4952,7 +4953,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4975,13 +4976,13 @@
         <v>44</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -5032,7 +5033,7 @@
         <v>44</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>42</v>
@@ -5047,7 +5048,7 @@
         <v>63</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AK33" t="s" s="2">
         <v>132</v>
@@ -5064,7 +5065,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5087,19 +5088,19 @@
         <v>44</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="O34" t="s" s="2">
         <v>44</v>
@@ -5148,7 +5149,7 @@
         <v>44</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>42</v>
@@ -5163,10 +5164,10 @@
         <v>63</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AL34" t="s" s="2">
         <v>44</v>
@@ -5180,7 +5181,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5206,10 +5207,10 @@
         <v>53</v>
       </c>
       <c r="K35" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="L35" t="s" s="2">
-        <v>227</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5260,7 +5261,7 @@
         <v>44</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>42</v>
@@ -5292,7 +5293,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5318,10 +5319,10 @@
         <v>96</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>230</v>
-      </c>
-      <c r="L36" t="s" s="2">
-        <v>231</v>
       </c>
       <c r="M36" t="s" s="2">
         <v>112</v>
@@ -5374,7 +5375,7 @@
         <v>44</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>42</v>
@@ -5406,11 +5407,11 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
@@ -5432,10 +5433,10 @@
         <v>96</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>235</v>
-      </c>
-      <c r="L37" t="s" s="2">
-        <v>236</v>
       </c>
       <c r="M37" t="s" s="2">
         <v>112</v>
@@ -5490,7 +5491,7 @@
         <v>44</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>42</v>
@@ -5522,7 +5523,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5545,19 +5546,19 @@
         <v>44</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>44</v>
@@ -5606,7 +5607,7 @@
         <v>44</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>51</v>
@@ -5621,16 +5622,16 @@
         <v>63</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AL38" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>44</v>
@@ -5638,7 +5639,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5664,16 +5665,16 @@
         <v>125</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>44</v>
@@ -5722,7 +5723,7 @@
         <v>44</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>42</v>
@@ -5737,16 +5738,16 @@
         <v>63</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>44</v>
@@ -5754,11 +5755,11 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
@@ -5777,16 +5778,16 @@
         <v>44</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
@@ -5836,7 +5837,7 @@
         <v>44</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>42</v>
@@ -5851,7 +5852,7 @@
         <v>63</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AK40" t="s" s="2">
         <v>132</v>
@@ -5860,7 +5861,7 @@
         <v>44</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>44</v>
@@ -5868,7 +5869,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5891,19 +5892,19 @@
         <v>52</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>44</v>
@@ -5952,7 +5953,7 @@
         <v>44</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>42</v>
@@ -5967,10 +5968,10 @@
         <v>63</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>44</v>
@@ -5984,7 +5985,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6007,19 +6008,19 @@
         <v>52</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="O42" t="s" s="2">
         <v>44</v>
@@ -6068,7 +6069,7 @@
         <v>44</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>42</v>
@@ -6083,7 +6084,7 @@
         <v>63</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AK42" t="s" s="2">
         <v>132</v>
@@ -6100,7 +6101,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6126,10 +6127,10 @@
         <v>53</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="L43" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="L43" t="s" s="2">
-        <v>227</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -6180,7 +6181,7 @@
         <v>44</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>42</v>
@@ -6212,7 +6213,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6238,10 +6239,10 @@
         <v>96</v>
       </c>
       <c r="K44" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>230</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>231</v>
       </c>
       <c r="M44" t="s" s="2">
         <v>112</v>
@@ -6294,7 +6295,7 @@
         <v>44</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>42</v>
@@ -6326,11 +6327,11 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
@@ -6352,10 +6353,10 @@
         <v>96</v>
       </c>
       <c r="K45" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="L45" t="s" s="2">
         <v>235</v>
-      </c>
-      <c r="L45" t="s" s="2">
-        <v>236</v>
       </c>
       <c r="M45" t="s" s="2">
         <v>112</v>
@@ -6410,7 +6411,7 @@
         <v>44</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>42</v>
@@ -6442,7 +6443,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6465,16 +6466,16 @@
         <v>52</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
@@ -6524,7 +6525,7 @@
         <v>44</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>51</v>
@@ -6548,7 +6549,7 @@
         <v>44</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>44</v>
@@ -6556,7 +6557,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6582,10 +6583,10 @@
         <v>71</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -6615,10 +6616,10 @@
         <v>157</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="Z47" t="s" s="2">
         <v>44</v>
@@ -6636,7 +6637,7 @@
         <v>44</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>51</v>
@@ -6651,7 +6652,7 @@
         <v>63</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="AK47" t="s" s="2">
         <v>132</v>

</xml_diff>